<commit_message>
Update Case_Studies.ipynb with case_study1 from Readme
</commit_message>
<xml_diff>
--- a/case_study1.xlsx
+++ b/case_study1.xlsx
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>337.6</v>
+        <v>354.5</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>315.4</v>
+        <v>342.3</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>335.9</v>
+        <v>340.7</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>321.6</v>
+        <v>300.2</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>288.5</v>
+        <v>305.1</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>306.4</v>
+        <v>295.3</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>379.1</v>
+        <v>389.9</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -566,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>381.3</v>
+        <v>419.3</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>360.4</v>
+        <v>326.2</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -600,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>325.1</v>
+        <v>343.1</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>336.4</v>
+        <v>336.7</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -634,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>291.7</v>
+        <v>311.1</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -651,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>465.4</v>
+        <v>402.9</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>409</v>
+        <v>417.8</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>402.2</v>
+        <v>396.3</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>417.2</v>
+        <v>424.2</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>395.2</v>
+        <v>318.7</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>365.1</v>
+        <v>345.9</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>442.6</v>
+        <v>435.1</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -770,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>435.1</v>
+        <v>417.2</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>447.2</v>
+        <v>437.6</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -804,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>423.1</v>
+        <v>466.3</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -821,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>414.7</v>
+        <v>434.6</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>439.2</v>
+        <v>426.9</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>525.3</v>
+        <v>521.5</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -872,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>496.9</v>
+        <v>518.5</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>454.7</v>
+        <v>475.9</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -906,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>454.7</v>
+        <v>449</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>432.4</v>
+        <v>512.9</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -940,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>460</v>
+        <v>465.4</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>

</xml_diff>